<commit_message>
add snc user query test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044p8f\Downloads\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A924B54F-5521-4AA1-9971-408E798BCEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9920E0D1-00B2-433A-9D71-3716423A594E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="98">
   <si>
     <t>description</t>
   </si>
@@ -222,62 +222,7 @@
     <t>schema</t>
   </si>
   <si>
-    <t>{
-    Product_Order(cond: "{ demand_date:{_gte: \"2020-10-01 00:00:00\"} }"){
-        insert_time
-        demand_date
-        sales_order
-    }
-}</t>
-  </si>
-  <si>
     <t>data.Product_Order</t>
-  </si>
-  <si>
-    <t>{
-    Product_Order(cond: "{ sales_order:{_eq: \"800014035899\"} }"){
-        sales_order
-        invert_Product {
-            product_no
-        }
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    Product_Order(cond: "{ demand_date:{_gte: \"2020-10-01 00:00:00\"} }") {
-        demand_date
-        insert_time
-        product
-        sales_order
-        invert_Product {
-            product_no
-            invert_Preactor_Order(cond: "{ start_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") {
-                order_no
-                product
-                plan_quantity
-                invert_Product_Order_Process(cond: "{ mach_type:{_eq:\"MPM******\"}, event_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") {
-                    product_order
-                    product
-                    pass_quantity
-                    produce_quantity
-                }
-            }
-            produced_Product_Qualification(cond: "{ mach_type:{_eq:\"MPM******\"}, event_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") {
-                test_result
-                product
-                mach_type
-                event_time
-                fid
-                invert_Production_Procedure {
-                    Work_On_Work_Position {
-                        work_center_id
-                    }
-                }
-            }
-        }
-    }
-}</t>
   </si>
   <si>
     <t>{
@@ -588,42 +533,75 @@
     <t>SNC-ApiEngine-Test-9-3</t>
   </si>
   <si>
-    <t>{
-    Work_Center(cond: "{ id:{_eq:\"9999999\"} }") {
-        id
-        field_not_exist
-    }
-}</t>
-  </si>
-  <si>
     <t>Field 'field_not_exist' in type 'Work_Center' is undefined</t>
   </si>
   <si>
-    <t>{
-    Work_Center(cond:"{not_exist:{_eq:\"23\"}}",order:"") {
-        id
-    }
-}</t>
-  </si>
-  <si>
     <t>Column 'not_exist' not found in any table</t>
   </si>
   <si>
     <t>SNC-ApiEngine-Test-9-4</t>
   </si>
   <si>
-    <t>{
-    Work_Center(cond: "{ id:{_eq:\"70000\"} }") {
-        id
-        Has_Preactor_Order(cond: "{ start_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") {
-            order_no
-            field_not_exist
+    <t>Field 'field_not_exist' in type 'Preactor_Order' is undefined</t>
+  </si>
+  <si>
+    <t>{ Product_Order(cond: "{ demand_date:{_gte: \"2020-10-01 00:00:00\"} }") {
+        insert_time
+        demand_date
+        sales_order
+}}</t>
+  </si>
+  <si>
+    <t>{ Product_Order(cond: "{ demand_date:{_gte: \"2020-10-01 00:00:00\"} }") {
+        demand_date
+        insert_time
+        product
+        sales_order
+        invert_Product {
+            product_no
+            invert_Preactor_Order(cond: "{ start_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") {
+                order_no
+                product
+                plan_quantity
+                invert_Product_Order_Process(cond: "{ mach_type:{_eq:\"MPM******\"}, event_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") {
+                    product_order
+                    product
+                    pass_quantity
+                    produce_quantity
+                }
+            }
+            produced_Product_Qualification(cond: "{ mach_type:{_eq:\"MPM******\"}, event_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") {
+                test_result
+                product
+                mach_type
+                event_time
+                fid
+                invert_Production_Procedure {
+                    Work_On_Work_Position {
+                        work_center_id
+                    }
+                }
+            }
         }
     }
 }</t>
   </si>
   <si>
-    <t>Field 'field_not_exist' in type 'Preactor_Order' is undefined</t>
+    <t>{ Product_Order(cond: "{ sales_order:{_eq: \"800014035899\"} }") {
+        sales_order
+        invert_Product { 
+            product_no 
+        }
+}}</t>
+  </si>
+  <si>
+    <t>{ Work_Center(cond: "{ id:{_eq:\"9999999\"} }") { id field_not_exist }}</t>
+  </si>
+  <si>
+    <t>{ Work_Center(cond:"{not_exist:{_eq:\"23\"}}",order:"") { id }}</t>
+  </si>
+  <si>
+    <t>{ Work_Center(cond: "{ id:{_eq:\"70000\"} }") { id Has_Preactor_Order(cond: "{ start_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") { order_no field_not_exist } } }</t>
   </si>
 </sst>
 </file>
@@ -652,7 +630,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -662,6 +640,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -704,6 +688,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,15 +976,15 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="1"/>
-    <col min="4" max="4" width="36.6640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.6640625" style="1"/>
+    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" style="1"/>
+    <col min="4" max="4" width="36.6328125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1025,7 +1010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1049,7 +1034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1073,7 +1058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1099,7 +1084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1123,7 +1108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1147,7 +1132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1171,7 +1156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1195,7 +1180,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1219,7 +1204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1254,19 +1239,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.6328125" style="6" customWidth="1"/>
+    <col min="4" max="5" width="12.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.81640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1286,7 +1272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1304,7 +1290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>20</v>
@@ -1322,7 +1308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -1340,7 +1326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -1358,7 +1344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>21</v>
@@ -1376,15 +1362,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D7" s="3">
         <v>200</v>
@@ -1393,18 +1379,18 @@
         <v>101301</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D8" s="3">
         <v>200</v>
@@ -1413,18 +1399,18 @@
         <v>101403</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="138" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3">
         <v>200</v>
@@ -1433,7 +1419,7 @@
         <v>101301</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1445,20 +1431,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33428B76-3520-4B33-A399-174FF1F65645}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="68.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1471,99 +1460,156 @@
       <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="3">
+        <v>200</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="138" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="E5" s="3">
+        <v>200</v>
+      </c>
+      <c r="F5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>89</v>
+      <c r="E6" s="3">
+        <v>200</v>
+      </c>
+      <c r="F6" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C236C6A-A34F-4BA7-95CF-30837F8A7B9E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1576,56 +1622,86 @@
       <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="8">
+        <v>200</v>
+      </c>
+      <c r="F2" s="8">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="386.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A91664E-6F1E-4B1F-8BD3-3809CECDC69D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E1" sqref="E1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1638,62 +1714,86 @@
       <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="8">
+        <v>200</v>
+      </c>
+      <c r="F2" s="8">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4A5408-F209-41F3-990B-0A79A152C374}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1706,64 +1806,109 @@
       <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="372.6" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="386.4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="E2" s="8">
+        <v>200</v>
+      </c>
+      <c r="F2" s="8">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="386.4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="E4" s="8">
+        <v>200</v>
+      </c>
+      <c r="F4" s="8">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="400.2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>200</v>
+      </c>
+      <c r="F5" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1771,13 +1916,22 @@
         <v>45</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="E6" s="8">
+        <v>200</v>
+      </c>
+      <c r="F6" s="8">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
@@ -1785,13 +1939,23 @@
         <v>47</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="E7" s="8">
+        <v>200</v>
+      </c>
+      <c r="F7" s="8">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix test data for snc-api-engine-test-9-3
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9920E0D1-00B2-433A-9D71-3716423A594E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870E77B5-5C3F-4E06-98EB-B5532A1859A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -536,9 +536,6 @@
     <t>Field 'field_not_exist' in type 'Work_Center' is undefined</t>
   </si>
   <si>
-    <t>Column 'not_exist' not found in any table</t>
-  </si>
-  <si>
     <t>SNC-ApiEngine-Test-9-4</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t>{ Work_Center(cond: "{ id:{_eq:\"70000\"} }") { id Has_Preactor_Order(cond: "{ start_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") { order_no field_not_exist } } }</t>
+  </si>
+  <si>
+    <t>Column 'NOT_EXIST' not found in any table</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="3">
         <v>200</v>
@@ -1390,7 +1390,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="3">
         <v>200</v>
@@ -1399,18 +1399,18 @@
         <v>101403</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="3">
         <v>200</v>
@@ -1419,7 +1419,7 @@
         <v>101301</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1475,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>50</v>
@@ -1498,7 +1498,7 @@
         <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>50</v>
@@ -1521,7 +1521,7 @@
         <v>55</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>50</v>
@@ -1780,7 +1780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4A5408-F209-41F3-990B-0A79A152C374}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix snc user query test - Materials JSON template update
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870E77B5-5C3F-4E06-98EB-B5532A1859A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79A6462-69DC-4461-9CD1-877178A9235A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
   <si>
     <t>description</t>
   </si>
@@ -503,12 +503,6 @@
     <t>SncPreactorOrder6.JSON</t>
   </si>
   <si>
-    <t>SncMaterial1.JSON</t>
-  </si>
-  <si>
-    <t>SncMaterial2.JSON</t>
-  </si>
-  <si>
     <t>SncWorkCenter1.JSON</t>
   </si>
   <si>
@@ -602,6 +596,9 @@
   </si>
   <si>
     <t>Column 'NOT_EXIST' not found in any table</t>
+  </si>
+  <si>
+    <t>SncMaterial.JSON</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1370,7 +1367,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D7" s="3">
         <v>200</v>
@@ -1379,18 +1376,18 @@
         <v>101301</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="3">
         <v>200</v>
@@ -1399,18 +1396,18 @@
         <v>101403</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D9" s="3">
         <v>200</v>
@@ -1419,7 +1416,7 @@
         <v>101301</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1475,13 +1472,13 @@
         <v>53</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -1498,13 +1495,13 @@
         <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="3">
         <v>200</v>
@@ -1521,13 +1518,13 @@
         <v>55</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="3">
         <v>200</v>
@@ -1550,7 +1547,7 @@
         <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="3">
         <v>200</v>
@@ -1573,7 +1570,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E6" s="3">
         <v>200</v>
@@ -1596,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C236C6A-A34F-4BA7-95CF-30837F8A7B9E}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1643,7 +1640,7 @@
         <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E2" s="8">
         <v>200</v>
@@ -1666,7 +1663,7 @@
         <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="E3" s="3">
         <v>200</v>
@@ -1735,7 +1732,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="8">
         <v>200</v>
@@ -1758,7 +1755,7 @@
         <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" s="3">
         <v>200</v>

</xml_diff>

<commit_message>
add case to check snc portal realtime function
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0424CDC-E0FF-4AA5-AD72-F4F8E59B4CF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A78251-B65F-4373-A66A-D1CB891336F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="queryMaterialByGraphQL" sheetId="7" r:id="rId4"/>
     <sheet name="queryWorkCenterByGraphQL" sheetId="6" r:id="rId5"/>
     <sheet name="queryPreactorOrderByGraphQL" sheetId="8" r:id="rId6"/>
+    <sheet name="queryCrestWelderByGraphQL" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="101">
   <si>
     <t>description</t>
   </si>
@@ -600,30 +601,138 @@
   <si>
     <t>SncMaterial.JSON</t>
   </si>
+  <si>
+    <t>jsonpath</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNC-ApiEngine-Test-10-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+        SINAMICS_300_LogConnection(cond: "{update_time:{_gte:\"$gteData\", _lte: \"$lteData\"}, port:{_eq:4}, sinamics_300:{_eq:\"9d734276-3a63-4bb7-a737-beb63b15e868\"}}", order: "update_time DESC", after: "0", first: 5) {
+          totalElements
+          totalPages
+          pageSize
+          page
+          numberOfElements
+          edges {
+            node {
+              outputcurrent_actual_AI0
+              Braking_status_word
+              input_current_actual_AI0
+              input_current_actual_AI1
+              Act_filtered_DC_link_volt
+              Safely_remove_mem_card_status
+              Actual_speed_smoothed
+              Motor_utilization_thermal
+              Number_of_drive_objects
+              id
+              port1_CO_motor_temperature
+              Fault_code_6
+              sinamics_300
+              Fault_code_5
+              Fault_code_8
+              Fault_code_7
+              Status_word_1
+              Pulse_frequency_Mod_min_value
+              Status_word_2
+              Digital_in_status_inverted
+              CO_Act_filtered_current_Isq
+              Status_word_faults_alarms_2
+              Energy_consumpt_meter
+              Status_word_faults_alarms_1
+              Converter_state
+              Device_type_identification
+              Device_Firmware_version
+              Analog_inputs_in_percent_AI1
+              Missing_enable_sig
+              unit_line_supply_voltage
+              Speed_setpoint_smoothed
+              port
+              Analog_inputs_in_percent_AI0
+              Firmware_date_year
+              Firmware_patch_hot_fix
+              terminal_actual_value
+              CO_Act_motor_temperature
+              S6_load_duty_cycle
+              Company_IDDeviceidentification
+              Rated_converter_power
+              Rated_converter_current
+              Firmware_date_day_month
+              Abs_actual_current_smoothed
+              ZSW_seq_ctrlStatuswordsequence
+              S1_cont_duty_cycle
+              update_time
+              Energy_consumption_saved
+              CU_Firmware_version
+              Freq_Setpoint_before_RFG
+              Digital_out_status
+              Pulse_frequency_Actual
+              Fault_code_2
+              Fault_code_1
+              Act_filtered_output_voltage
+              Fault_code_4
+              Fault_code_3
+              Act_filtered_frequency
+              Act_filtered_rotor_speed
+              Digital_in_status
+              Act_filtered_torque
+              output_current_actual_AI1
+              Actual_alarm_code
+              Act_filtered_powerDisplays
+              Rated_motor_current
+              CO_Converter_temperature
+              Control_word_faults_alarms
+              Actual_fault_code
+              Control_word_1
+            }
+            cursor
+          }
+          pageInfo {
+            endCursor
+            hasNextPage
+          }
+        }
+      }</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>data.SINAMICS_300_LogConnection.totalElements</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -973,7 +1082,7 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1"/>
@@ -981,7 +1090,7 @@
     <col min="5" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1031,7 +1140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1055,7 +1164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1081,7 +1190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1105,7 +1214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1129,7 +1238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1153,7 +1262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1177,7 +1286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1236,11 +1345,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
@@ -1249,7 +1358,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1269,7 +1378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1287,7 +1396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>20</v>
@@ -1305,7 +1414,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -1323,7 +1432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -1341,7 +1450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>21</v>
@@ -1359,7 +1468,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
@@ -1379,7 +1488,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>85</v>
       </c>
@@ -1399,7 +1508,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>87</v>
       </c>
@@ -1435,7 +1544,7 @@
       <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="68.77734375" style="1" customWidth="1"/>
@@ -1444,7 +1553,7 @@
     <col min="5" max="7" width="12.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1467,7 +1576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -1490,7 +1599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>54</v>
       </c>
@@ -1513,7 +1622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>55</v>
       </c>
@@ -1536,7 +1645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>56</v>
       </c>
@@ -1559,7 +1668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
@@ -1597,7 +1706,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -1606,7 +1715,7 @@
     <col min="5" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1629,7 +1738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
@@ -1652,7 +1761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -1676,6 +1785,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1689,7 +1799,7 @@
       <selection activeCell="E1" sqref="E1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -1698,7 +1808,7 @@
     <col min="5" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1721,7 +1831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -1744,7 +1854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>61</v>
       </c>
@@ -1768,6 +1878,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1781,7 +1892,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
@@ -1790,7 +1901,7 @@
     <col min="5" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1813,7 +1924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
@@ -1836,7 +1947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
@@ -1859,7 +1970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
@@ -1882,7 +1993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -1905,7 +2016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1928,7 +2039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
@@ -1952,6 +2063,67 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5B1355-72F0-4004-98DD-807F072B7A8E}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="8">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update not_exist into lowercase
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/snc-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A78251-B65F-4373-A66A-D1CB891336F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A583D159-7178-4C97-817C-35999BBA4993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="13800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -594,9 +594,6 @@
   </si>
   <si>
     <t>{ Work_Center(cond: "{ id:{_eq:\"70000\"} }") { id Has_Preactor_Order(cond: "{ start_time:{_gte:\"2020-10-01 00:00:00\", _lt:\"2020-10-02 00:00:00\"} }") { order_no field_not_exist } } }</t>
-  </si>
-  <si>
-    <t>Column 'NOT_EXIST' not found in any table</t>
   </si>
   <si>
     <t>SncMaterial.JSON</t>
@@ -701,6 +698,10 @@
   <si>
     <t>data.SINAMICS_300_LogConnection.totalElements</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Column ‘not_exist' not found in any table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1345,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1506,7 @@
         <v>101403</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
@@ -1749,7 +1750,7 @@
         <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="8">
         <v>200</v>
@@ -1772,7 +1773,7 @@
         <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="3">
         <v>200</v>
@@ -2073,7 +2074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5B1355-72F0-4004-98DD-807F072B7A8E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2090,7 +2091,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -2104,13 +2105,13 @@
     </row>
     <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="D2" s="8">
         <v>200</v>

</xml_diff>